<commit_message>
Updated Biodiversity Bulk Upload and AddDataManually
</commit_message>
<xml_diff>
--- a/WMIS/Content/Files/BiodiversityBulkUploadTemplate.xlsx
+++ b/WMIS/Content/Files/BiodiversityBulkUploadTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Family</t>
-  </si>
-  <si>
-    <t>Status Rank</t>
   </si>
 </sst>
 </file>
@@ -249,7 +246,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,12 +441,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,7 +680,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -708,7 +699,6 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="97">
     <cellStyle name="20 % - Accent1 2" xfId="68"/>
@@ -1106,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK128"/>
+  <dimension ref="A1:AJ128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1108,7 @@
     <col min="13" max="13" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1161,16 +1151,13 @@
       <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>17</v>
+      <c r="O1" t="s">
+        <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1180,8 +1167,8 @@
     <row r="38" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J38" s="2"/>
     </row>
-    <row r="128" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK128" s="2"/>
+    <row r="128" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ128" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>